<commit_message>
Implemented select channel to preview
</commit_message>
<xml_diff>
--- a/template/BDEW.xlsx
+++ b/template/BDEW.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="157">
   <si>
     <t>Condition</t>
   </si>
@@ -53,15 +53,24 @@
     <t>dd.mm.yyyy</t>
   </si>
   <si>
+    <t>B1</t>
+  </si>
+  <si>
     <t>Time</t>
   </si>
   <si>
     <t>hh:mm:ss.f</t>
   </si>
   <si>
+    <t>B2</t>
+  </si>
+  <si>
     <t>Type of fault</t>
   </si>
   <si>
+    <t>B3</t>
+  </si>
+  <si>
     <t>Drop depth setpoint</t>
   </si>
   <si>
@@ -71,40 +80,73 @@
     <t>p.u.</t>
   </si>
   <si>
+    <t>B4</t>
+  </si>
+  <si>
     <t>Drop duration setpoint</t>
   </si>
   <si>
     <t>ms</t>
   </si>
   <si>
+    <t>B5</t>
+  </si>
+  <si>
     <t>Value of the sries impedance X1, if applicable</t>
   </si>
   <si>
     <t>Ω</t>
   </si>
   <si>
+    <t>B6</t>
+  </si>
+  <si>
     <t>Value of the series impedance R1, if applicable</t>
   </si>
   <si>
+    <t>B7</t>
+  </si>
+  <si>
     <t>Value of the short-circuit impedance X2, if applicable</t>
   </si>
   <si>
+    <t>B8</t>
+  </si>
+  <si>
     <t>Value of the short-circuit impedance R2, if applicable</t>
   </si>
   <si>
+    <t>B9</t>
+  </si>
+  <si>
     <t>Connection series impedance(t0), if applicable</t>
   </si>
   <si>
+    <t>B10</t>
+  </si>
+  <si>
     <t>Fault occurrence (t1)</t>
   </si>
   <si>
+    <t>B11</t>
+  </si>
+  <si>
     <t>Fault clearance (t2)</t>
   </si>
   <si>
+    <t>B12</t>
+  </si>
+  <si>
     <t>Bridging series impedance (t3), if applicable</t>
   </si>
   <si>
+    <t>B13</t>
+  </si>
+  <si>
     <t>Fault duration determined from test</t>
+  </si>
+  <si>
+    <t>B14</t>
   </si>
   <si>
     <t>Actual value of voltage drop / increase</t>
@@ -114,12 +156,21 @@
 t1 - 60 s to t1</t>
   </si>
   <si>
+    <t>B15</t>
+  </si>
+  <si>
     <t>pos</t>
   </si>
   <si>
+    <t>B16</t>
+  </si>
+  <si>
     <t>neg</t>
   </si>
   <si>
+    <t>B17</t>
+  </si>
+  <si>
     <t>Before t0</t>
   </si>
   <si>
@@ -129,44 +180,101 @@
     <t>t0-500ms to t0-100ms</t>
   </si>
   <si>
+    <t>B18</t>
+  </si>
+  <si>
     <t>Current</t>
   </si>
   <si>
     <t>t0-500ms to to-100ms</t>
   </si>
   <si>
+    <t>B19</t>
+  </si>
+  <si>
     <t>Active power</t>
   </si>
   <si>
+    <t>B20</t>
+  </si>
+  <si>
     <t>Reactive power</t>
   </si>
   <si>
+    <t>B21</t>
+  </si>
+  <si>
     <t>Before dip &lt;t1</t>
   </si>
   <si>
     <t>t1 - 60 s to t1</t>
+  </si>
+  <si>
+    <t>B22</t>
+  </si>
+  <si>
+    <t>B23</t>
+  </si>
+  <si>
+    <t>B24</t>
   </si>
   <si>
     <t>t1 - 500 ms to 
 t1 - 100 ms</t>
   </si>
   <si>
+    <t>B25</t>
+  </si>
+  <si>
     <t>t1 - 1 s to t1</t>
   </si>
   <si>
+    <t>B26</t>
+  </si>
+  <si>
+    <t>B27</t>
+  </si>
+  <si>
+    <t>B28</t>
+  </si>
+  <si>
     <t>Reactive current</t>
   </si>
   <si>
+    <t>B29</t>
+  </si>
+  <si>
+    <t>B30</t>
+  </si>
+  <si>
+    <t>B31</t>
+  </si>
+  <si>
     <t>Active current</t>
   </si>
   <si>
+    <t>B32</t>
+  </si>
+  <si>
     <t>total</t>
   </si>
   <si>
     <t>t1 - 10 s to t1</t>
   </si>
   <si>
+    <t>B33</t>
+  </si>
+  <si>
     <t>t1 - 2 s to t1</t>
+  </si>
+  <si>
+    <t>B34</t>
+  </si>
+  <si>
+    <t>B35</t>
+  </si>
+  <si>
+    <t>B36</t>
   </si>
   <si>
     <t>Wind speed
@@ -176,25 +284,73 @@
     <t>m/s</t>
   </si>
   <si>
+    <t>B37</t>
+  </si>
+  <si>
     <t>During dip t1 to t2</t>
   </si>
   <si>
     <t>Determined proportionality constant K-factor</t>
   </si>
   <si>
+    <t>B38</t>
+  </si>
+  <si>
+    <t>B39</t>
+  </si>
+  <si>
     <t>Reactive current settling up time</t>
   </si>
   <si>
+    <t>B40</t>
+  </si>
+  <si>
+    <t>B41</t>
+  </si>
+  <si>
     <t>Reactive current settling time</t>
+  </si>
+  <si>
+    <t>B42</t>
+  </si>
+  <si>
+    <t>B43</t>
   </si>
   <si>
     <t>t1 + 100 ms to 
 t2 - 20ms</t>
   </si>
   <si>
+    <t>B44</t>
+  </si>
+  <si>
+    <t>B45</t>
+  </si>
+  <si>
+    <t>B46</t>
+  </si>
+  <si>
+    <t>B47</t>
+  </si>
+  <si>
+    <t>B48</t>
+  </si>
+  <si>
     <t>Apparent current</t>
   </si>
   <si>
+    <t>B49</t>
+  </si>
+  <si>
+    <t>B50</t>
+  </si>
+  <si>
+    <t>B51</t>
+  </si>
+  <si>
+    <t>B52</t>
+  </si>
+  <si>
     <t>Line current</t>
   </si>
   <si>
@@ -207,28 +363,91 @@
     <t>A</t>
   </si>
   <si>
+    <t>B53</t>
+  </si>
+  <si>
     <t>Phase 2</t>
   </si>
   <si>
+    <t>B54</t>
+  </si>
+  <si>
     <t>Phase 3</t>
   </si>
   <si>
+    <t>B55</t>
+  </si>
+  <si>
     <t>t1 + 20 ms</t>
   </si>
   <si>
+    <t>B56</t>
+  </si>
+  <si>
+    <t>B57</t>
+  </si>
+  <si>
+    <t>B58</t>
+  </si>
+  <si>
     <t>t1 + 100 ms</t>
   </si>
   <si>
+    <t>B59</t>
+  </si>
+  <si>
+    <t>B60</t>
+  </si>
+  <si>
+    <t>B61</t>
+  </si>
+  <si>
     <t>t1 + 150 ms</t>
   </si>
   <si>
+    <t>B62</t>
+  </si>
+  <si>
+    <t>B63</t>
+  </si>
+  <si>
+    <t>B64</t>
+  </si>
+  <si>
     <t>t1 + 300 ms</t>
   </si>
   <si>
+    <t>B65</t>
+  </si>
+  <si>
+    <t>B66</t>
+  </si>
+  <si>
+    <t>B67</t>
+  </si>
+  <si>
     <t>t1 + 500 ms</t>
   </si>
   <si>
+    <t>B68</t>
+  </si>
+  <si>
+    <t>B69</t>
+  </si>
+  <si>
+    <t>B70</t>
+  </si>
+  <si>
     <t>t1 + 1000 ms</t>
+  </si>
+  <si>
+    <t>B71</t>
+  </si>
+  <si>
+    <t>B72</t>
+  </si>
+  <si>
+    <t>B73</t>
   </si>
   <si>
     <t>After dip
@@ -238,22 +457,37 @@
     <t>t2 + 1 s to t2 + 10 s</t>
   </si>
   <si>
+    <t>B74</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
+    <t>B75</t>
+  </si>
+  <si>
     <t>Wind speed (WT only)</t>
   </si>
   <si>
     <t>t2+1s to t2+10s</t>
   </si>
   <si>
+    <t>B76</t>
+  </si>
+  <si>
     <t>Active current rise time</t>
   </si>
   <si>
     <t>s</t>
   </si>
   <si>
+    <t>B77</t>
+  </si>
+  <si>
     <t>Rective current rise time</t>
+  </si>
+  <si>
+    <t>B78</t>
   </si>
 </sst>
 </file>
@@ -273,7 +507,6 @@
     </font>
     <font/>
     <font>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -289,7 +522,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border/>
     <border>
       <left style="thin">
@@ -335,11 +568,16 @@
         <color rgb="FF000000"/>
       </right>
     </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -355,10 +593,16 @@
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,7 +889,9 @@
       <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="5"/>
@@ -653,7 +899,7 @@
         <v>3.0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
@@ -662,9 +908,11 @@
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5"/>
@@ -672,7 +920,7 @@
         <v>4.0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -683,7 +931,9 @@
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5"/>
@@ -691,18 +941,20 @@
         <v>5.0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="5"/>
@@ -710,7 +962,7 @@
         <v>6.0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -719,9 +971,11 @@
         <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5"/>
@@ -729,7 +983,7 @@
         <v>7.0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -738,9 +992,11 @@
         <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5"/>
@@ -748,7 +1004,7 @@
         <v>8.0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
@@ -757,9 +1013,11 @@
         <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5"/>
@@ -767,7 +1025,7 @@
         <v>9.0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>10</v>
@@ -776,9 +1034,11 @@
         <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5"/>
@@ -786,7 +1046,7 @@
         <v>10.0</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>10</v>
@@ -795,9 +1055,11 @@
         <v>10</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5"/>
@@ -805,7 +1067,7 @@
         <v>11.0</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>10</v>
@@ -814,9 +1076,11 @@
         <v>10</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5"/>
@@ -824,7 +1088,7 @@
         <v>12.0</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>10</v>
@@ -833,9 +1097,11 @@
         <v>10</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5"/>
@@ -843,7 +1109,7 @@
         <v>13.0</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>10</v>
@@ -852,9 +1118,11 @@
         <v>10</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="5"/>
@@ -862,7 +1130,7 @@
         <v>14.0</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>10</v>
@@ -871,9 +1139,11 @@
         <v>10</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5"/>
@@ -881,7 +1151,7 @@
         <v>15.0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>10</v>
@@ -890,9 +1160,11 @@
         <v>10</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="5"/>
@@ -900,18 +1172,20 @@
         <v>16.0</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5"/>
@@ -920,11 +1194,13 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="4"/>
@@ -933,32 +1209,36 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B21" s="7">
         <v>19.0</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="5"/>
@@ -966,18 +1246,20 @@
         <v>20.0</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5"/>
@@ -985,18 +1267,20 @@
         <v>21.0</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="4"/>
@@ -1004,39 +1288,43 @@
         <v>22.0</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B25" s="7">
         <v>23.0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="5"/>
@@ -1045,13 +1333,15 @@
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5"/>
@@ -1060,13 +1350,15 @@
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="F27" s="5"/>
-      <c r="G27" s="6"/>
+      <c r="G27" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="5"/>
@@ -1075,13 +1367,15 @@
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="6"/>
+      <c r="G28" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5"/>
@@ -1090,13 +1384,15 @@
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F29" s="5"/>
-      <c r="G29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5"/>
@@ -1105,13 +1401,15 @@
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="6"/>
+      <c r="G30" s="6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5"/>
@@ -1119,18 +1417,20 @@
         <v>29.0</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="5"/>
@@ -1138,18 +1438,20 @@
         <v>30.0</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5"/>
@@ -1158,13 +1460,15 @@
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F33" s="5"/>
-      <c r="G33" s="6"/>
+      <c r="G33" s="6" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="5"/>
@@ -1173,13 +1477,15 @@
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F34" s="4"/>
-      <c r="G34" s="6"/>
+      <c r="G34" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5"/>
@@ -1187,18 +1493,20 @@
         <v>33.0</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="5"/>
@@ -1206,18 +1514,20 @@
         <v>34.0</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5"/>
@@ -1226,13 +1536,15 @@
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="3" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="F37" s="5"/>
-      <c r="G37" s="6"/>
+      <c r="G37" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5"/>
@@ -1241,13 +1553,15 @@
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="F38" s="4"/>
-      <c r="G38" s="6"/>
+      <c r="G38" s="6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="5"/>
@@ -1255,18 +1569,20 @@
         <v>37.0</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="4"/>
@@ -1274,31 +1590,33 @@
         <v>38.0</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G40" s="6"/>
+        <v>88</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B41" s="7">
         <v>39.0</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>10</v>
@@ -1306,7 +1624,9 @@
       <c r="F41" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G41" s="6"/>
+      <c r="G41" s="6" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="5"/>
@@ -1315,7 +1635,7 @@
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>10</v>
@@ -1323,7 +1643,9 @@
       <c r="F42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G42" s="6"/>
+      <c r="G42" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="5"/>
@@ -1331,18 +1653,20 @@
         <v>41.0</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="5"/>
@@ -1351,13 +1675,15 @@
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F44" s="4"/>
-      <c r="G44" s="6"/>
+      <c r="G44" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="5"/>
@@ -1365,18 +1691,20 @@
         <v>43.0</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="5"/>
@@ -1385,13 +1713,15 @@
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F46" s="4"/>
-      <c r="G46" s="6"/>
+      <c r="G46" s="6" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="5"/>
@@ -1399,18 +1729,20 @@
         <v>45.0</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="5"/>
@@ -1419,11 +1751,13 @@
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
-      <c r="G48" s="6"/>
+      <c r="G48" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="5"/>
@@ -1432,11 +1766,13 @@
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="6"/>
+      <c r="G49" s="6" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="5"/>
@@ -1444,18 +1780,20 @@
         <v>48.0</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="5"/>
@@ -1464,11 +1802,13 @@
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
-      <c r="G51" s="6"/>
+      <c r="G51" s="6" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="5"/>
@@ -1476,18 +1816,20 @@
         <v>50.0</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G52" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="5"/>
@@ -1496,11 +1838,13 @@
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="6"/>
+      <c r="G53" s="6" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="5"/>
@@ -1508,18 +1852,20 @@
         <v>52.0</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G54" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="5"/>
@@ -1528,11 +1874,13 @@
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="6"/>
+      <c r="G55" s="6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="5"/>
@@ -1540,18 +1888,20 @@
         <v>54.0</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G56" s="6"/>
+        <v>114</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="5"/>
@@ -1560,11 +1910,13 @@
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="3" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
-      <c r="G57" s="6"/>
+      <c r="G57" s="6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="5"/>
@@ -1573,11 +1925,13 @@
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="3" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="6"/>
+      <c r="G58" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="5"/>
@@ -1585,18 +1939,20 @@
         <v>57.0</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="5"/>
@@ -1605,11 +1961,13 @@
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="3" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
-      <c r="G60" s="6"/>
+      <c r="G60" s="6" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="5"/>
@@ -1618,11 +1976,13 @@
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="3" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="6"/>
+      <c r="G61" s="6" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="5"/>
@@ -1631,15 +1991,17 @@
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="3" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G62" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="5"/>
@@ -1648,11 +2010,13 @@
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="3" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
-      <c r="G63" s="6"/>
+      <c r="G63" s="6" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="5"/>
@@ -1661,11 +2025,13 @@
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="3" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="6"/>
+      <c r="G64" s="6" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="5"/>
@@ -1674,15 +2040,17 @@
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="3" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G65" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="5"/>
@@ -1691,11 +2059,13 @@
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="3" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
-      <c r="G66" s="6"/>
+      <c r="G66" s="6" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="5"/>
@@ -1704,11 +2074,13 @@
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="3" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
-      <c r="G67" s="6"/>
+      <c r="G67" s="6" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="5"/>
@@ -1717,15 +2089,17 @@
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="3" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G68" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="5"/>
@@ -1734,11 +2108,13 @@
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="3" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="6"/>
+      <c r="G69" s="6" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="5"/>
@@ -1747,11 +2123,13 @@
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="3" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
-      <c r="G70" s="6"/>
+      <c r="G70" s="6" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="5"/>
@@ -1760,15 +2138,17 @@
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="3" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G71" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="5"/>
@@ -1777,11 +2157,13 @@
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="3" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
-      <c r="G72" s="6"/>
+      <c r="G72" s="6" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="5"/>
@@ -1790,11 +2172,13 @@
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="3" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
-      <c r="G73" s="6"/>
+      <c r="G73" s="6" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="5"/>
@@ -1803,15 +2187,17 @@
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="3" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G74" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="5"/>
@@ -1820,11 +2206,13 @@
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="3" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
-      <c r="G75" s="6"/>
+      <c r="G75" s="6" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="4"/>
@@ -1833,32 +2221,36 @@
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="3" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="6"/>
+      <c r="G76" s="6" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="B77" s="7">
         <v>75.0</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G77" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="5"/>
@@ -1866,18 +2258,20 @@
         <v>76.0</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G78" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="5"/>
@@ -1885,18 +2279,20 @@
         <v>77.0</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G79" s="6"/>
+        <v>88</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="5"/>
@@ -1904,18 +2300,20 @@
         <v>78.0</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G80" s="6"/>
+        <v>153</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="4"/>
@@ -1923,12 +2321,17 @@
         <v>79.0</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
-      <c r="G81" s="6"/>
+      <c r="G81" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="G82" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="52">

</xml_diff>